<commit_message>
Ajustes para conseguir rodar sem a base full e de alguns erros. Envio do arquivo utilizando "read_fwf".
</commit_message>
<xml_diff>
--- a/dados/LAYOUT_DADOS_ABERTOS_CNPJ.xlsx
+++ b/dados/LAYOUT_DADOS_ABERTOS_CNPJ.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22920"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22930"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Programas\R\Projects\Fundacoes\dados\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Programas\R\Projects\R_Base_CNPJ_RF\dados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D3A1C94-932F-4682-8534-9D1EAF091B18}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD37BE3B-A015-454B-8341-295935CC09CF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="460" xr2:uid="{EB4C5E13-ECED-4D90-8A9E-F96664C4D839}"/>
+    <workbookView xWindow="-20610" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="450" xr2:uid="{EB4C5E13-ECED-4D90-8A9E-F96664C4D839}"/>
   </bookViews>
   <sheets>
     <sheet name="Layout_CNPJ_RF" sheetId="3" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Layout_CNPJ_RF!$A$1:$J$91</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Layout_CNPJ_RF!$A$1:$K$91</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -530,14 +530,14 @@
     <t>RAZÃO SOCIAL-NOME EMPRESARIAL</t>
   </si>
   <si>
-    <t>RegistroDoido</t>
+    <t>Ver1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -555,6 +555,14 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -598,7 +606,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -619,6 +627,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -952,12 +961,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C2FE000-8794-4742-941A-36F773E5911D}">
-  <dimension ref="A1:K91"/>
+  <dimension ref="A1:M91"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="J1" sqref="D1:J1048576"/>
+      <selection pane="bottomLeft" activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -966,15 +975,16 @@
     <col min="2" max="2" width="16.7109375" customWidth="1"/>
     <col min="3" max="3" width="8.7109375" hidden="1" customWidth="1"/>
     <col min="4" max="4" width="20.5703125" style="6" customWidth="1"/>
-    <col min="5" max="6" width="20.42578125" customWidth="1"/>
+    <col min="5" max="5" width="20.42578125" customWidth="1"/>
+    <col min="6" max="6" width="7.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="6.7109375" customWidth="1"/>
-    <col min="8" max="8" width="17.28515625" customWidth="1"/>
-    <col min="9" max="9" width="29" style="6" customWidth="1"/>
+    <col min="8" max="8" width="6.42578125" customWidth="1"/>
+    <col min="9" max="9" width="13.7109375" style="6" customWidth="1"/>
     <col min="10" max="10" width="18.85546875" customWidth="1"/>
     <col min="11" max="11" width="18.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1008,8 +1018,9 @@
       <c r="K1" s="3" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="M1" s="10"/>
+    </row>
+    <row r="2" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -1037,7 +1048,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" ht="90" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -1071,7 +1082,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -1101,7 +1112,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -1131,7 +1142,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -1161,7 +1172,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" ht="180" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -1191,7 +1202,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -1221,7 +1232,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -1251,7 +1262,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>26</v>
       </c>
@@ -1279,7 +1290,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" ht="90" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>26</v>
       </c>
@@ -1309,7 +1320,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>26</v>
       </c>
@@ -1339,7 +1350,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>26</v>
       </c>
@@ -1369,7 +1380,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" ht="120" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>26</v>
       </c>
@@ -1399,7 +1410,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>26</v>
       </c>
@@ -1429,7 +1440,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>26</v>
       </c>
@@ -1459,7 +1470,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>26</v>
       </c>
@@ -1489,7 +1500,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" ht="135" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>26</v>
       </c>
@@ -1519,7 +1530,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>26</v>
       </c>
@@ -1549,7 +1560,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>26</v>
       </c>
@@ -1579,7 +1590,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>26</v>
       </c>
@@ -1609,7 +1620,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>26</v>
       </c>
@@ -1639,7 +1650,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>26</v>
       </c>
@@ -1669,7 +1680,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>26</v>
       </c>
@@ -1699,7 +1710,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>26</v>
       </c>
@@ -1729,7 +1740,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" ht="105" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>26</v>
       </c>
@@ -1759,7 +1770,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>26</v>
       </c>
@@ -1789,7 +1800,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" ht="120" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>26</v>
       </c>
@@ -1819,7 +1830,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:11" ht="90" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" ht="195" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>26</v>
       </c>
@@ -1849,7 +1860,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" ht="135" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>26</v>
       </c>
@@ -1879,7 +1890,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>26</v>
       </c>
@@ -1909,7 +1920,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" ht="150" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>26</v>
       </c>
@@ -1939,7 +1950,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" ht="120" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>26</v>
       </c>
@@ -1969,7 +1980,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" ht="135" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>26</v>
       </c>
@@ -1999,7 +2010,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" ht="120" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>26</v>
       </c>
@@ -2272,7 +2283,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>26</v>
       </c>
@@ -2302,7 +2313,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>26</v>
       </c>
@@ -2332,7 +2343,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>26</v>
       </c>
@@ -2362,7 +2373,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" ht="165" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>26</v>
       </c>
@@ -2392,7 +2403,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" ht="180" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>26</v>
       </c>
@@ -2422,7 +2433,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>26</v>
       </c>
@@ -2452,7 +2463,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>26</v>
       </c>
@@ -2482,7 +2493,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" ht="135" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>26</v>
       </c>
@@ -2512,7 +2523,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>26</v>
       </c>
@@ -2542,7 +2553,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>26</v>
       </c>
@@ -2602,7 +2613,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>26</v>
       </c>
@@ -2632,7 +2643,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>107</v>
       </c>
@@ -2662,7 +2673,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="58" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11" ht="105" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>107</v>
       </c>
@@ -2692,7 +2703,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="59" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>107</v>
       </c>
@@ -2722,7 +2733,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="60" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>107</v>
       </c>
@@ -2752,7 +2763,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="61" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:11" ht="120" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>107</v>
       </c>
@@ -2782,7 +2793,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="62" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>107</v>
       </c>
@@ -2812,7 +2823,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="63" spans="1:11" ht="105" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:11" ht="240" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>107</v>
       </c>
@@ -2842,7 +2853,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="64" spans="1:11" ht="105" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:11" ht="255" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>107</v>
       </c>
@@ -2872,7 +2883,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="65" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>107</v>
       </c>
@@ -2902,7 +2913,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="66" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:11" ht="105" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>107</v>
       </c>
@@ -2932,7 +2943,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="67" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>107</v>
       </c>
@@ -2962,7 +2973,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="68" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:11" ht="105" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>107</v>
       </c>
@@ -2992,7 +3003,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="69" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:11" ht="105" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>107</v>
       </c>
@@ -3022,7 +3033,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="70" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>107</v>
       </c>
@@ -3052,7 +3063,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="71" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>107</v>
       </c>
@@ -3082,7 +3093,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="72" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:11" ht="105" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>107</v>
       </c>
@@ -3142,7 +3153,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="74" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>107</v>
       </c>
@@ -3172,7 +3183,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="75" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>136</v>
       </c>
@@ -3202,7 +3213,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="76" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>136</v>
       </c>
@@ -3232,7 +3243,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="77" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:11" ht="180" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>136</v>
       </c>
@@ -3262,7 +3273,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="78" spans="1:11" ht="150" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:11" ht="345" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>136</v>
       </c>
@@ -3292,7 +3303,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="79" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:11" ht="120" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>136</v>
       </c>
@@ -3322,7 +3333,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="80" spans="1:11" ht="135" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:11" ht="285" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>136</v>
       </c>
@@ -3385,7 +3396,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="82" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>136</v>
       </c>
@@ -3415,7 +3426,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="83" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>143</v>
       </c>
@@ -3442,7 +3453,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="84" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>143</v>
       </c>
@@ -3472,7 +3483,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="85" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>143</v>
       </c>
@@ -3502,7 +3513,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="86" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>143</v>
       </c>
@@ -3532,7 +3543,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="87" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>143</v>
       </c>
@@ -3562,7 +3573,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="88" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>143</v>
       </c>
@@ -3592,7 +3603,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="89" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:11" ht="105" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>143</v>
       </c>
@@ -3652,7 +3663,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="91" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>143</v>
       </c>
@@ -3683,7 +3694,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J91" xr:uid="{2DEC433A-923B-497F-B075-421139A20040}"/>
+  <autoFilter ref="A1:K91" xr:uid="{579ABDCB-722E-4F0E-97E7-15BC424A20BD}"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
@@ -3691,12 +3702,11 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_Flow_SignoffStatus xmlns="e461758b-926b-44e9-b618-2ebbf9c7904c" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3923,17 +3933,27 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_Flow_SignoffStatus xmlns="e461758b-926b-44e9-b618-2ebbf9c7904c" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{27974B32-D619-4D50-9978-F80B18AAF86A}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3861DCC3-C013-4624-8CA5-C523409E6909}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="e461758b-926b-44e9-b618-2ebbf9c7904c"/>
+    <ds:schemaRef ds:uri="5b029b56-3411-473c-8dc4-47702cfa7f09"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3958,18 +3978,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3861DCC3-C013-4624-8CA5-C523409E6909}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{27974B32-D619-4D50-9978-F80B18AAF86A}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="e461758b-926b-44e9-b618-2ebbf9c7904c"/>
-    <ds:schemaRef ds:uri="5b029b56-3411-473c-8dc4-47702cfa7f09"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>